<commit_message>
se agrego el diseno final
</commit_message>
<xml_diff>
--- a/Proyecto RISCV32/Instrucciones/Control_Unit.xlsx
+++ b/Proyecto RISCV32/Instrucciones/Control_Unit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TEC\2022\II Semestre 2022\Microprocesadores y Microcontroladores\git\Proyecto RISCV32\Instrucciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nadir's PC\Documents\TEC\Microprocesadores y microcontroladores\Proyecto2022\Proyecto RISCV32\Instrucciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5957DE3E-6BE3-4755-98BA-C93DC7274DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6F1700-BFB9-4626-9259-0D78FB41793C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{86A48E26-F327-4EB6-89F6-4A7C5D4D33BE}"/>
+    <workbookView xWindow="-120" yWindow="-45" windowWidth="25845" windowHeight="15435" xr2:uid="{86A48E26-F327-4EB6-89F6-4A7C5D4D33BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="55">
   <si>
     <t>I-type</t>
   </si>
@@ -149,9 +149,6 @@
     <t>100</t>
   </si>
   <si>
-    <t>extendUn</t>
-  </si>
-  <si>
     <t>suma</t>
   </si>
   <si>
@@ -164,13 +161,43 @@
     <t>1</t>
   </si>
   <si>
-    <t>extiende de 12 a 32 bits</t>
-  </si>
-  <si>
     <t>AND</t>
   </si>
   <si>
-    <t>extiende de ? a 32 bits</t>
+    <t>Lreg</t>
+  </si>
+  <si>
+    <t>WeMem</t>
+  </si>
+  <si>
+    <t>00</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Operacion</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Byte</t>
+  </si>
+  <si>
+    <t>Leer</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Revisado</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -396,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -467,19 +494,17 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -491,29 +516,25 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -530,7 +551,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -828,11 +849,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA29F1A3-E384-4B00-829D-01A4F2B3AA1F}">
   <dimension ref="A1:CH2979"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK21" sqref="AK21"/>
+    <sheetView tabSelected="1" topLeftCell="Y9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AH9" sqref="AH9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
@@ -972,7 +993,7 @@
         <v>21</v>
       </c>
       <c r="AO1" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="AP1" s="4"/>
       <c r="AQ1" s="8"/>
@@ -1037,34 +1058,34 @@
       <c r="K2" s="35"/>
       <c r="L2" s="35"/>
       <c r="M2" s="35"/>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="33" t="s">
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="34" t="s">
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="31" t="s">
+      <c r="W2" s="42"/>
+      <c r="X2" s="42"/>
+      <c r="Y2" s="42"/>
+      <c r="Z2" s="42"/>
+      <c r="AA2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="31"/>
+      <c r="AB2" s="41"/>
+      <c r="AC2" s="41"/>
+      <c r="AD2" s="41"/>
+      <c r="AE2" s="41"/>
+      <c r="AF2" s="41"/>
+      <c r="AG2" s="41"/>
       <c r="AH2" s="5"/>
       <c r="AI2" s="18"/>
       <c r="AJ2" s="17"/>
@@ -1072,8 +1093,8 @@
       <c r="AL2" s="2"/>
       <c r="AM2" s="2"/>
       <c r="AN2" s="2"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="41"/>
+      <c r="AO2" s="30"/>
+      <c r="AP2" s="32"/>
       <c r="AQ2" s="21"/>
       <c r="AR2" s="21"/>
       <c r="AS2" s="21"/>
@@ -1226,21 +1247,23 @@
         <v>17</v>
       </c>
       <c r="AK3" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL3" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM3" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN3" s="2">
         <v>1</v>
       </c>
-      <c r="AO3" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="41"/>
+      <c r="AO3" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP3" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ3" s="21"/>
       <c r="AR3" s="21"/>
       <c r="AS3" s="21"/>
@@ -1393,21 +1416,23 @@
         <v>17</v>
       </c>
       <c r="AK4" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL4" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM4" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM4" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN4" s="2">
         <v>1</v>
       </c>
-      <c r="AO4" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="41"/>
+      <c r="AO4" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP4" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ4" s="21"/>
       <c r="AR4" s="21"/>
       <c r="AS4" s="21"/>
@@ -1560,21 +1585,23 @@
         <v>17</v>
       </c>
       <c r="AK5" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM5" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM5" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN5" s="2">
         <v>1</v>
       </c>
-      <c r="AO5" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="41"/>
+      <c r="AO5" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP5" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ5" s="21"/>
       <c r="AR5" s="21"/>
       <c r="AS5" s="21"/>
@@ -1727,21 +1754,23 @@
         <v>17</v>
       </c>
       <c r="AK6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL6" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM6" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM6" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN6" s="2">
         <v>1</v>
       </c>
-      <c r="AO6" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="41"/>
+      <c r="AO6" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP6" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ6" s="21"/>
       <c r="AR6" s="21"/>
       <c r="AS6" s="21"/>
@@ -1894,21 +1923,23 @@
         <v>17</v>
       </c>
       <c r="AK7" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM7" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM7" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN7" s="2">
         <v>1</v>
       </c>
-      <c r="AO7" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="41"/>
+      <c r="AO7" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP7" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ7"/>
       <c r="AR7"/>
       <c r="AS7"/>
@@ -2061,21 +2092,23 @@
         <v>17</v>
       </c>
       <c r="AK8" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM8" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM8" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN8" s="2">
         <v>1</v>
       </c>
-      <c r="AO8" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="41"/>
+      <c r="AO8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP8" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ8"/>
       <c r="AR8"/>
       <c r="AS8"/>
@@ -2228,21 +2261,23 @@
         <v>17</v>
       </c>
       <c r="AK9" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM9" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM9" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN9" s="2">
         <v>1</v>
       </c>
-      <c r="AO9" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="41"/>
+      <c r="AO9" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP9" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ9"/>
       <c r="AR9"/>
       <c r="AS9"/>
@@ -2395,21 +2430,23 @@
         <v>18</v>
       </c>
       <c r="AK10" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AL10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM10" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM10" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN10" s="2">
         <v>1</v>
       </c>
-      <c r="AO10" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="41"/>
+      <c r="AO10" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ10"/>
       <c r="AR10"/>
       <c r="AS10"/>
@@ -2562,21 +2599,23 @@
         <v>18</v>
       </c>
       <c r="AK11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AL11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM11" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM11" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN11" s="2">
         <v>1</v>
       </c>
-      <c r="AO11" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="41"/>
+      <c r="AO11" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ11"/>
       <c r="AR11"/>
       <c r="AS11"/>
@@ -2729,21 +2768,23 @@
         <v>18</v>
       </c>
       <c r="AK12" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AL12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM12" s="2">
-        <v>0</v>
+        <v>40</v>
+      </c>
+      <c r="AM12" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN12" s="2">
         <v>1</v>
       </c>
-      <c r="AO12" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP12" s="41"/>
+      <c r="AO12" s="30">
+        <v>1</v>
+      </c>
+      <c r="AP12" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
@@ -2853,21 +2894,23 @@
         <v>17</v>
       </c>
       <c r="AK13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL13" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="AL13" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AM13" s="2">
-        <v>0</v>
+      <c r="AM13" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="AN13" s="2">
         <v>1</v>
       </c>
-      <c r="AO13" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP13" s="41"/>
+      <c r="AO13" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP13" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:85" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
@@ -2911,7 +2954,7 @@
       <c r="AM14" s="5"/>
       <c r="AN14" s="5"/>
       <c r="AO14" s="5"/>
-      <c r="AP14" s="41"/>
+      <c r="AP14" s="32"/>
     </row>
     <row r="15" spans="1:85" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
@@ -2933,34 +2976,34 @@
       <c r="K15" s="37"/>
       <c r="L15" s="37"/>
       <c r="M15" s="37"/>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="33" t="s">
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="T15" s="33"/>
-      <c r="U15" s="33"/>
-      <c r="V15" s="30" t="s">
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="W15" s="30"/>
-      <c r="X15" s="30"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="31" t="s">
+      <c r="W15" s="40"/>
+      <c r="X15" s="40"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AB15" s="31"/>
-      <c r="AC15" s="31"/>
-      <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
-      <c r="AF15" s="31"/>
-      <c r="AG15" s="31"/>
+      <c r="AB15" s="41"/>
+      <c r="AC15" s="41"/>
+      <c r="AD15" s="41"/>
+      <c r="AE15" s="41"/>
+      <c r="AF15" s="41"/>
+      <c r="AG15" s="41"/>
       <c r="AH15" s="5"/>
       <c r="AI15" s="18"/>
       <c r="AJ15" s="17"/>
@@ -2968,8 +3011,8 @@
       <c r="AL15" s="2"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
-      <c r="AO15" s="39"/>
-      <c r="AP15" s="41"/>
+      <c r="AO15" s="30"/>
+      <c r="AP15" s="32"/>
       <c r="AQ15"/>
       <c r="AR15"/>
       <c r="AS15"/>
@@ -3121,22 +3164,24 @@
       <c r="AJ16" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AK16" s="2">
-        <v>0</v>
+      <c r="AK16" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AL16" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM16" s="2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="AM16" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="AN16" s="2">
         <v>0</v>
       </c>
-      <c r="AO16" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP16" s="41"/>
+      <c r="AO16" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP16" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="17" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -3245,22 +3290,24 @@
       <c r="AJ17" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AK17" s="2">
-        <v>0</v>
+      <c r="AK17" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AL17" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM17" s="2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="AM17" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="AN17" s="2">
         <v>0</v>
       </c>
-      <c r="AO17" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP17" s="41"/>
+      <c r="AO17" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP17" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:86" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -3369,22 +3416,24 @@
       <c r="AJ18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AK18" s="2">
-        <v>0</v>
+      <c r="AK18" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AL18" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM18" s="2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="AM18" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="AN18" s="2">
         <v>0</v>
       </c>
-      <c r="AO18" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP18" s="41"/>
+      <c r="AO18" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP18" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ18"/>
       <c r="AR18"/>
       <c r="AS18"/>
@@ -3537,22 +3586,24 @@
       <c r="AJ19" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AK19" s="2">
-        <v>0</v>
+      <c r="AK19" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AL19" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM19" s="2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="AM19" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="AN19" s="2">
         <v>0</v>
       </c>
-      <c r="AO19" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP19" s="41"/>
+      <c r="AO19" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP19" s="32" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="20" spans="1:86" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -3661,22 +3712,24 @@
       <c r="AJ20" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="AK20" s="2">
-        <v>0</v>
+      <c r="AK20" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="AL20" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM20" s="2">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="AM20" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="AN20" s="2">
         <v>0</v>
       </c>
-      <c r="AO20" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP20" s="41"/>
+      <c r="AO20" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP20" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="AQ20"/>
       <c r="AR20"/>
       <c r="AS20"/>
@@ -3764,7 +3817,7 @@
       <c r="AM21" s="5"/>
       <c r="AN21" s="5"/>
       <c r="AO21" s="5"/>
-      <c r="AP21" s="41"/>
+      <c r="AP21" s="32"/>
       <c r="AQ21"/>
       <c r="AR21"/>
       <c r="AS21"/>
@@ -4111,19 +4164,21 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="25"/>
       <c r="AJ25" s="25"/>
-      <c r="AK25" s="24"/>
-      <c r="AL25" s="40" t="s">
+      <c r="AK25" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL25" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="AM25" s="39" t="s">
-        <v>40</v>
+      <c r="AM25" s="30" t="s">
+        <v>39</v>
       </c>
       <c r="AN25" s="24"/>
-      <c r="AO25" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP25" s="42" t="s">
-        <v>40</v>
+      <c r="AO25" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP25" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="AQ25"/>
       <c r="AR25"/>
@@ -4166,9 +4221,7 @@
       <c r="CC25"/>
       <c r="CD25"/>
       <c r="CE25"/>
-      <c r="CF25"/>
-      <c r="CG25"/>
-      <c r="CH25" s="20"/>
+      <c r="CF25" s="20"/>
     </row>
     <row r="26" spans="1:86" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
@@ -4208,18 +4261,18 @@
       <c r="AI26" s="25"/>
       <c r="AJ26" s="25"/>
       <c r="AK26" s="24"/>
-      <c r="AL26" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM26" s="39" t="s">
-        <v>39</v>
+      <c r="AL26" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM26" s="30" t="s">
+        <v>38</v>
       </c>
       <c r="AN26" s="24"/>
-      <c r="AO26" s="39">
-        <v>0</v>
-      </c>
-      <c r="AP26" s="42" t="s">
-        <v>43</v>
+      <c r="AO26" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP26" s="31" t="s">
+        <v>51</v>
       </c>
       <c r="AQ26"/>
       <c r="AR26"/>
@@ -4262,9 +4315,7 @@
       <c r="CC26"/>
       <c r="CD26"/>
       <c r="CE26"/>
-      <c r="CF26"/>
-      <c r="CG26"/>
-      <c r="CH26" s="20"/>
+      <c r="CF26" s="20"/>
     </row>
     <row r="27" spans="1:86" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
@@ -4304,18 +4355,18 @@
       <c r="AI27" s="25"/>
       <c r="AJ27" s="25"/>
       <c r="AK27" s="24"/>
-      <c r="AL27" s="43" t="s">
+      <c r="AL27" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM27" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="AM27" s="44" t="s">
-        <v>44</v>
-      </c>
       <c r="AN27" s="24"/>
-      <c r="AO27" s="39">
-        <v>1</v>
-      </c>
-      <c r="AP27" s="42" t="s">
-        <v>45</v>
+      <c r="AO27" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP27" s="31" t="s">
+        <v>49</v>
       </c>
       <c r="AQ27"/>
       <c r="AR27"/>
@@ -4358,9 +4409,7 @@
       <c r="CC27"/>
       <c r="CD27"/>
       <c r="CE27"/>
-      <c r="CF27"/>
-      <c r="CG27"/>
-      <c r="CH27" s="20"/>
+      <c r="CF27" s="20"/>
     </row>
     <row r="28" spans="1:86" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
@@ -4400,11 +4449,15 @@
       <c r="AI28" s="25"/>
       <c r="AJ28" s="25"/>
       <c r="AK28" s="24"/>
-      <c r="AL28" s="45"/>
-      <c r="AM28" s="38"/>
+      <c r="AL28" s="25"/>
+      <c r="AM28" s="24"/>
       <c r="AN28" s="24"/>
-      <c r="AO28" s="24"/>
-      <c r="AP28"/>
+      <c r="AO28" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="AP28" s="31" t="s">
+        <v>50</v>
+      </c>
       <c r="AQ28"/>
       <c r="AR28"/>
       <c r="AS28"/>
@@ -4488,10 +4541,10 @@
       <c r="AI29" s="25"/>
       <c r="AJ29" s="25"/>
       <c r="AK29" s="24"/>
-      <c r="AL29" s="45"/>
-      <c r="AM29" s="38"/>
+      <c r="AL29" s="25"/>
+      <c r="AM29" s="24"/>
       <c r="AN29" s="24"/>
-      <c r="AO29" s="24"/>
+      <c r="AO29" s="43"/>
       <c r="AP29"/>
       <c r="AQ29"/>
       <c r="AR29"/>
@@ -17006,17 +17059,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="I15:M15"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="S15:U15"/>
     <mergeCell ref="V15:Z15"/>
     <mergeCell ref="AA15:AG15"/>
     <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="N2:R2"/>
     <mergeCell ref="S2:U2"/>
     <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="I15:M15"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="S15:U15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>